<commit_message>
Atualização automática de SANTO_ANGELO.xlsx
</commit_message>
<xml_diff>
--- a/SANTO_ANGELO.xlsx
+++ b/SANTO_ANGELO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C7EDAA14-0AC9-4840-B556-5BF57B6C5F90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{60DECB6A-1DEE-4E95-9C16-89C50D931055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1241,7 +1241,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{F292B155-F21F-409C-BC44-2280F7A473A5}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{F7947B21-D840-4241-9723-2F7109A6F84D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1271,10 +1271,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F08BFCEB-7700-4CD5-9AC9-B5F5BFBB7278}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{451BBF06-D33A-4224-9E6A-CADAA61C014D}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1312,7 +1312,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00E9A800-3C03-4EBF-9F82-B38FB2241B72}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{103AD7C5-565E-4D1F-BB73-3FCA80468E00}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1375,7 +1375,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F3A4A14-3E59-4E0B-B85C-77A3ACFAC940}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2660DF0B-67C8-4686-AE82-2EAA60C550E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1394,7 +1394,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{729528CC-6E66-F704-38AF-E46D0772506C}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5F4EB2E-9840-D36C-F671-D18D8F46C97E}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1443,7 +1443,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F57CF181-D054-D50F-63A9-21141A7A6A8F}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2908D0BB-7954-122C-15D3-B4E67C4CDDA3}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1462,7 +1462,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{443FC028-1EA3-609D-3C95-F71B8E63E4A6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{85DBB007-4CC1-B58B-00C2-E5D0D9A8ACA6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1493,7 +1493,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A56B8D68-6E4C-A80B-FEB9-8EF623DBADE1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{527489BF-7551-59E4-FE4A-80D68D61A4CF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1524,7 +1524,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED358A15-FE01-57F7-4964-819349D4A4CD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95C07531-68B1-601C-6956-8840E79DD4EC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1567,7 +1567,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10625913-BF75-4E8F-A4F8-B8DE0DE57AB2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CFB7E75-5C27-4769-AF8C-440FA15923C2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1605,7 +1605,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8B27A756-FDAB-46B6-BFD7-8E86654FD4FE}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26E42571-7DF7-44ED-B92F-7E484F96801A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1648,7 +1648,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84DBEE00-9E40-4AC3-B4B1-13C25B88194F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A06E16B5-CA56-4998-8DCC-6B5143366C7B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1961,7 +1961,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CA1531-F872-4AD4-BDFB-CC937E0AD6DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1BDD485-31A9-43B8-82D3-78697AA44B92}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>